<commit_message>
changed names for us national accounts and usecon
</commit_message>
<xml_diff>
--- a/data/processing/haver_names.xlsx
+++ b/data/processing/haver_names.xlsx
@@ -8,19 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malcalakovalski\Documents\Fiscal-Impact-Measure\data\processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAA1D8D-ACC5-467F-80B8-CA0215B938A7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6280FBE-1241-4BD6-8E53-F9261EDCA659}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="75" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="National Accounts Quarterly" sheetId="1" r:id="rId1"/>
+    <sheet name="National Accounts Annual" sheetId="5" r:id="rId2"/>
+    <sheet name="USECON Quarterly" sheetId="2" r:id="rId3"/>
+    <sheet name="USECON Annual" sheetId="6" r:id="rId4"/>
+    <sheet name="Descriptions" sheetId="3" r:id="rId5"/>
+    <sheet name="Sources" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sources!$A$1:$D$46</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="237">
   <si>
     <t>code</t>
   </si>
@@ -310,7 +329,427 @@
     <t>transfersUnemploymentState</t>
   </si>
   <si>
-    <t>date</t>
+    <t>Quartely</t>
+  </si>
+  <si>
+    <t>GDP</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>GDPH</t>
+  </si>
+  <si>
+    <t>JC</t>
+  </si>
+  <si>
+    <t>JGDP</t>
+  </si>
+  <si>
+    <t>JGF</t>
+  </si>
+  <si>
+    <t>JGS</t>
+  </si>
+  <si>
+    <t>JGSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State &amp; Local Govt Consumption Expenditures: Chn Price Index(SA, 2012=100) </t>
+  </si>
+  <si>
+    <t>JGSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State &amp; Local Govt Gross Investment: Chn Price Index(SA, 2012=100) </t>
+  </si>
+  <si>
+    <t>PTGH</t>
+  </si>
+  <si>
+    <t>PTGSH</t>
+  </si>
+  <si>
+    <t>PTGFH</t>
+  </si>
+  <si>
+    <t>YPTMR</t>
+  </si>
+  <si>
+    <t>YPTMD</t>
+  </si>
+  <si>
+    <t>YPTU</t>
+  </si>
+  <si>
+    <t>GTFP</t>
+  </si>
+  <si>
+    <t>YPOG</t>
+  </si>
+  <si>
+    <t>YPTX</t>
+  </si>
+  <si>
+    <t>YTPI</t>
+  </si>
+  <si>
+    <t>YCTLG</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>GRCSI</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>GF</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>GFH</t>
+  </si>
+  <si>
+    <t>GSH</t>
+  </si>
+  <si>
+    <t>GFRPT</t>
+  </si>
+  <si>
+    <t>GFRPRI</t>
+  </si>
+  <si>
+    <t>GFRCP</t>
+  </si>
+  <si>
+    <t>GFRS</t>
+  </si>
+  <si>
+    <t>GFTFP</t>
+  </si>
+  <si>
+    <t>GFEG</t>
+  </si>
+  <si>
+    <t>GSRPT</t>
+  </si>
+  <si>
+    <t>GSRPRI</t>
+  </si>
+  <si>
+    <t>GSRCP</t>
+  </si>
+  <si>
+    <t>GSRS</t>
+  </si>
+  <si>
+    <t>GSTFP</t>
+  </si>
+  <si>
+    <t>GSET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State &amp; Local Government Total Expenditures (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t>GFEGHHX</t>
+  </si>
+  <si>
+    <t>GFEGHDX</t>
+  </si>
+  <si>
+    <t>GFEIGX</t>
+  </si>
+  <si>
+    <t>Federal Investment Grants to State and Local Govenments (SAAR, Mil.$)</t>
+  </si>
+  <si>
+    <t>GFSUB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal Government Subsidies (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t>GSSUB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State and Local Government Subsidies (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t>GSUB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government Subsidies (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t>PCW</t>
+  </si>
+  <si>
+    <t>GDPPOTHQ</t>
+  </si>
+  <si>
+    <t>GDPPOTQ</t>
+  </si>
+  <si>
+    <t>RECESSQ</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>YP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal Income (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t>USPHPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAFH House Price Index: Purchase Only, United States (SA, Q1 1991-100) </t>
+  </si>
+  <si>
+    <t>CASUSXAM</t>
+  </si>
+  <si>
+    <t>S&amp;P CoreLogic Case-Shiller Home Price Index: US National (SA, Jan-00=100)</t>
+  </si>
+  <si>
+    <t>GDPPOT</t>
+  </si>
+  <si>
+    <t>Potential Gross Domestic Product [CBO] (Bil.$)]</t>
+  </si>
+  <si>
+    <t>GDPPOTH</t>
+  </si>
+  <si>
+    <t>Real Potential Gross Domestic Product [CBO] (Bil.Chn.2012$)</t>
+  </si>
+  <si>
+    <t>Variable Name / Haver Code</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>BEA Table</t>
+  </si>
+  <si>
+    <t>Raw Source for Historical Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross Domestic Product (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t>1.1.6</t>
+  </si>
+  <si>
+    <t>BEA, NIPAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal Consumption Expenditures (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Personal Consumption Expenditures (SAAR, Bil.Chn.2012.$) </t>
+  </si>
+  <si>
+    <t>1.1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Gross Domestic Product (SAAR, Bil.Chn.2012$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal Consumption Expenditures: Chain Price Index (SA, 2012=100) </t>
+  </si>
+  <si>
+    <t>1.1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross Domestic Product: Chain Price Index (SA, 2012=100) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal Govt Consumption &amp; Gross Investment: Chn Price Index(SA, 2012=100) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">State &amp; Local Govt Consumption/Gross Investment: Chn Price Index(SA, 2012=100) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government Social Benefit Payments to Persons: Medicare (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government Social Benefit Payments to Persons: Medicaid (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Govt Transf to Persons: Unemployment Insurance Benefits (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government Social Benefit Payments to Persons (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal Current Transfer Payments to Government (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal Current Taxes (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government Tax Receipts on Corporate Income (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government Consumption Expenditures &amp; Gross Investment (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t>gfrcf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal Govt Tax Rcpts on Corporate Income: Federal Reserve Banks (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contributions for Government Social Insurance (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal Consumption Expenditures: Implicit Price Deflator (SA, 2012=100) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal Government Consumption &amp; Gross Investment (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">State &amp; Local Government Consumption &amp; Gross Investment (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Federal Government Consumption &amp; Gross Investment (SAAR, Bil.Chn.2012$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real State &amp; Local Govt Consumption &amp; Gross Investment (SAAR, Bil.Chn.2012$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal Government Personal Current Tax Receipts (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal Government Tax Receipts on Corporate Income (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contributions for Federal Government Social Insurance (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal Government Social Benefit Payments to Persons (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal Grants-in-Aid to State &amp; Local Governments (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t>Federal grants-in-aid to state and local governments: Health and Hospitals (SAAR, Mil.$)</t>
+  </si>
+  <si>
+    <t>3.24U</t>
+  </si>
+  <si>
+    <t>BEA, NIPAS U</t>
+  </si>
+  <si>
+    <t>Federal grants-in-aid to state and local governments: Medicaid (SAAR, Mil.$)</t>
+  </si>
+  <si>
+    <t>gfiegx</t>
+  </si>
+  <si>
+    <t>Federal capital grants to state and local governments (SAAR, Mil.$)</t>
+  </si>
+  <si>
+    <t>5.11U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State &amp; Local Government Personal Current Tax Receipts (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">State &amp; Local Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">State &amp; Local Government Tax Receipts on Corporate Income (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contributions for State &amp; Local Government Social Insurance (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">State &amp; Local Government Social Benefit Payments to Persons (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government Consumption &amp; Investment: Contrib to Real GDP % Change (SAAR, %Pt) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">State &amp; Local Govt Consumption/Investment: Contrib to Real GDP % Chg (SAAR, %Pt) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal Govt Consumption &amp; Investment: Contrib to Real GDP % Change (SAAR, %Pt) </t>
+  </si>
+  <si>
+    <t>pcw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPI-W: All Items (SA, 1982-84=100) </t>
+  </si>
+  <si>
+    <t>BLS</t>
+  </si>
+  <si>
+    <t>gdppothq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Potential Gross Domestic Product [CBO] (SAAR, Bil.Chn.2012$) </t>
+  </si>
+  <si>
+    <t>CBO</t>
+  </si>
+  <si>
+    <t>gdppotq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential Gross Domestic Product [CBO] (SAAR, Bil.$) </t>
+  </si>
+  <si>
+    <t>recessq</t>
+  </si>
+  <si>
+    <t>Quarterly NBER Recession/Expansion: Recession Shading </t>
+  </si>
+  <si>
+    <t>NBER</t>
+  </si>
+  <si>
+    <t>cpiW</t>
+  </si>
+  <si>
+    <t>gdpPotential</t>
+  </si>
+  <si>
+    <t>gdpPotentialReal</t>
+  </si>
+  <si>
+    <t>recession</t>
+  </si>
+  <si>
+    <t>yp</t>
+  </si>
+  <si>
+    <t>personalIncome</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -359,7 +798,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -377,6 +816,641 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="VLOOKUP"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Variable Name / Haver Code</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>Description</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>BEA Table</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>Raw Source for Historical Data</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>gdp</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v xml:space="preserve">Gross Domestic Product (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C2" t="str">
+            <v>1.1.6</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>c</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v xml:space="preserve">Personal Consumption Expenditures (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>1.1.6</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>ch</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v xml:space="preserve">Real Personal Consumption Expenditures (SAAR, Bil.Chn.2012.$) </v>
+          </cell>
+          <cell r="C4" t="str">
+            <v>1.1.5</v>
+          </cell>
+          <cell r="D4" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>gdph</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v xml:space="preserve">Real Gross Domestic Product (SAAR, Bil.Chn.2012$) </v>
+          </cell>
+          <cell r="C5" t="str">
+            <v>1.1.5</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>jc</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v xml:space="preserve">Personal Consumption Expenditures: Chain Price Index (SA, 2012=100) </v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>1.1.4</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>jgdp</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v xml:space="preserve">Gross Domestic Product: Chain Price Index (SA, 2012=100) </v>
+          </cell>
+          <cell r="C7" t="str">
+            <v>1.1.4</v>
+          </cell>
+          <cell r="D7" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>jgf</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v xml:space="preserve">Federal Govt Consumption &amp; Gross Investment: Chn Price Index(SA, 2012=100) </v>
+          </cell>
+          <cell r="C8" t="str">
+            <v>1.1.4</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>jgs</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v xml:space="preserve">State &amp; Local Govt Consumption/Gross Investment: Chn Price Index(SA, 2012=100) </v>
+          </cell>
+          <cell r="C9" t="str">
+            <v>1.1.4</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>yptmr</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v xml:space="preserve">Government Social Benefit Payments to Persons: Medicare (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C10">
+            <v>2.1</v>
+          </cell>
+          <cell r="D10" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>yptmd</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v xml:space="preserve">Government Social Benefit Payments to Persons: Medicaid (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C11">
+            <v>2.1</v>
+          </cell>
+          <cell r="D11" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>yptu</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v xml:space="preserve">Govt Transf to Persons: Unemployment Insurance Benefits (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C12">
+            <v>2.1</v>
+          </cell>
+          <cell r="D12" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>gtfp</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v xml:space="preserve">Government Social Benefit Payments to Persons (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C13">
+            <v>3.1</v>
+          </cell>
+          <cell r="D13" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>ypog</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v xml:space="preserve">Personal Current Transfer Payments to Government (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C14">
+            <v>2.1</v>
+          </cell>
+          <cell r="D14" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>yptx</v>
+          </cell>
+          <cell r="B15" t="str">
+            <v xml:space="preserve">Personal Current Taxes (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C15">
+            <v>3.1</v>
+          </cell>
+          <cell r="D15" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>ytpi</v>
+          </cell>
+          <cell r="B16" t="str">
+            <v xml:space="preserve">Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C16">
+            <v>3.1</v>
+          </cell>
+          <cell r="D16" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>yctlg</v>
+          </cell>
+          <cell r="B17" t="str">
+            <v xml:space="preserve">Government Tax Receipts on Corporate Income (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C17">
+            <v>3.1</v>
+          </cell>
+          <cell r="D17" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>g</v>
+          </cell>
+          <cell r="B18" t="str">
+            <v xml:space="preserve">Government Consumption Expenditures &amp; Gross Investment (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C18" t="str">
+            <v>1.1.5</v>
+          </cell>
+          <cell r="D18" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>gfrcf</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v xml:space="preserve">Federal Govt Tax Rcpts on Corporate Income: Federal Reserve Banks (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="D19" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>grcsi</v>
+          </cell>
+          <cell r="B20" t="str">
+            <v xml:space="preserve">Contributions for Government Social Insurance (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="D20" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>dc</v>
+          </cell>
+          <cell r="B21" t="str">
+            <v xml:space="preserve">Personal Consumption Expenditures: Implicit Price Deflator (SA, 2012=100) </v>
+          </cell>
+          <cell r="C21">
+            <v>3.1</v>
+          </cell>
+          <cell r="D21" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>gf</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v xml:space="preserve">Federal Government Consumption &amp; Gross Investment (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C22" t="str">
+            <v>1.1.5</v>
+          </cell>
+          <cell r="D22" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>gs</v>
+          </cell>
+          <cell r="B23" t="str">
+            <v xml:space="preserve">State &amp; Local Government Consumption &amp; Gross Investment (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C23" t="str">
+            <v>1.1.5</v>
+          </cell>
+          <cell r="D23" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>gfh</v>
+          </cell>
+          <cell r="B24" t="str">
+            <v xml:space="preserve">Real Federal Government Consumption &amp; Gross Investment (SAAR, Bil.Chn.2012$) </v>
+          </cell>
+          <cell r="C24" t="str">
+            <v>1.1.6</v>
+          </cell>
+          <cell r="D24" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
+            <v>gsh</v>
+          </cell>
+          <cell r="B25" t="str">
+            <v xml:space="preserve">Real State &amp; Local Govt Consumption &amp; Gross Investment (SAAR, Bil.Chn.2012$) </v>
+          </cell>
+          <cell r="C25" t="str">
+            <v>1.1.6</v>
+          </cell>
+          <cell r="D25" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26" t="str">
+            <v>gfrpt</v>
+          </cell>
+          <cell r="B26" t="str">
+            <v xml:space="preserve">Federal Government Personal Current Tax Receipts (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C26">
+            <v>3.2</v>
+          </cell>
+          <cell r="D26" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>gfrpri</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v xml:space="preserve">Federal Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C27">
+            <v>3.2</v>
+          </cell>
+          <cell r="D27" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>gfrcp</v>
+          </cell>
+          <cell r="B28" t="str">
+            <v xml:space="preserve">Federal Government Tax Receipts on Corporate Income (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C28">
+            <v>3.2</v>
+          </cell>
+          <cell r="D28" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>gfrs</v>
+          </cell>
+          <cell r="B29" t="str">
+            <v xml:space="preserve">Contributions for Federal Government Social Insurance (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C29">
+            <v>3.2</v>
+          </cell>
+          <cell r="D29" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>gftfp</v>
+          </cell>
+          <cell r="B30" t="str">
+            <v xml:space="preserve">Federal Government Social Benefit Payments to Persons (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C30">
+            <v>3.2</v>
+          </cell>
+          <cell r="D30" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>gfeg</v>
+          </cell>
+          <cell r="B31" t="str">
+            <v xml:space="preserve">Federal Grants-in-Aid to State &amp; Local Governments (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C31">
+            <v>3.2</v>
+          </cell>
+          <cell r="D31" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>gfeghhx</v>
+          </cell>
+          <cell r="B32" t="str">
+            <v>Federal grants-in-aid to state and local governments: Health and Hospitals (SAAR, Mil.$)</v>
+          </cell>
+          <cell r="C32" t="str">
+            <v>3.24U</v>
+          </cell>
+          <cell r="D32" t="str">
+            <v>BEA, NIPAS U</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>gfeghdx</v>
+          </cell>
+          <cell r="B33" t="str">
+            <v>Federal grants-in-aid to state and local governments: Medicaid (SAAR, Mil.$)</v>
+          </cell>
+          <cell r="C33" t="str">
+            <v>3.24U</v>
+          </cell>
+          <cell r="D33" t="str">
+            <v>BEA, NIPAS U</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>gfiegx</v>
+          </cell>
+          <cell r="B34" t="str">
+            <v>Federal capital grants to state and local governments (SAAR, Mil.$)</v>
+          </cell>
+          <cell r="C34" t="str">
+            <v>5.11U</v>
+          </cell>
+          <cell r="D34" t="str">
+            <v>BEA, NIPAS U</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>gsrpt</v>
+          </cell>
+          <cell r="B35" t="str">
+            <v xml:space="preserve">State &amp; Local Government Personal Current Tax Receipts (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C35">
+            <v>3.3</v>
+          </cell>
+          <cell r="D35" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>gsrpri</v>
+          </cell>
+          <cell r="B36" t="str">
+            <v xml:space="preserve">State &amp; Local Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C36">
+            <v>3.3</v>
+          </cell>
+          <cell r="D36" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>gsrcp</v>
+          </cell>
+          <cell r="B37" t="str">
+            <v xml:space="preserve">State &amp; Local Government Tax Receipts on Corporate Income (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C37">
+            <v>3.3</v>
+          </cell>
+          <cell r="D37" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>gsrs</v>
+          </cell>
+          <cell r="B38" t="str">
+            <v xml:space="preserve">Contributions for State &amp; Local Government Social Insurance (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C38">
+            <v>3.3</v>
+          </cell>
+          <cell r="D38" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>gstfp</v>
+          </cell>
+          <cell r="B39" t="str">
+            <v xml:space="preserve">State &amp; Local Government Social Benefit Payments to Persons (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="C39">
+            <v>3.3</v>
+          </cell>
+          <cell r="D39" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>ptgh</v>
+          </cell>
+          <cell r="B40" t="str">
+            <v xml:space="preserve">Government Consumption &amp; Investment: Contrib to Real GDP % Change (SAAR, %Pt) </v>
+          </cell>
+          <cell r="D40" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>ptgsh</v>
+          </cell>
+          <cell r="B41" t="str">
+            <v xml:space="preserve">State &amp; Local Govt Consumption/Investment: Contrib to Real GDP % Chg (SAAR, %Pt) </v>
+          </cell>
+          <cell r="D41" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42" t="str">
+            <v>ptgfh</v>
+          </cell>
+          <cell r="B42" t="str">
+            <v xml:space="preserve">Federal Govt Consumption &amp; Investment: Contrib to Real GDP % Change (SAAR, %Pt) </v>
+          </cell>
+          <cell r="D42" t="str">
+            <v>BEA, NIPAS</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43" t="str">
+            <v>pcw</v>
+          </cell>
+          <cell r="B43" t="str">
+            <v xml:space="preserve">CPI-W: All Items (SA, 1982-84=100) </v>
+          </cell>
+          <cell r="D43" t="str">
+            <v>BLS</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44" t="str">
+            <v>gdppothq</v>
+          </cell>
+          <cell r="B44" t="str">
+            <v xml:space="preserve">Real Potential Gross Domestic Product [CBO] (SAAR, Bil.Chn.2012$) </v>
+          </cell>
+          <cell r="D44" t="str">
+            <v>CBO</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>gdppotq</v>
+          </cell>
+          <cell r="B45" t="str">
+            <v xml:space="preserve">Potential Gross Domestic Product [CBO] (SAAR, Bil.$) </v>
+          </cell>
+          <cell r="D45" t="str">
+            <v>CBO</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>recessq</v>
+          </cell>
+          <cell r="B46" t="str">
+            <v>Quarterly NBER Recession/Expansion: Recession Shading </v>
+          </cell>
+          <cell r="D46" t="str">
+            <v>NBER</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -700,10 +1774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,387 +1790,379 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>96</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B48" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>94</v>
-      </c>
-      <c r="B49" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1106,22 +2172,2045 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB820F1-8AA6-46BD-ABE0-EE31E37673CA}">
+  <dimension ref="A1:D37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="str">
+        <f>VLOOKUP(A1,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>reference</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>gdpNom</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>personalConsumptionNom</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="str">
+        <f>VLOOKUP(A4,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>personalConsumptionReal</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>gdpReal</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>personalConsumptionChain</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>gdpChain</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>consumptionInvestmentChainFederal</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="str">
+        <f>VLOOKUP(A9,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>consumptionInvestmentChainState</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="str">
+        <f>VLOOKUP(A10,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>socialBenefitsMedicare</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="str">
+        <f>VLOOKUP(A11,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>socialBenefitsMedicaid</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="str">
+        <f>VLOOKUP(A12,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>socialBenefits</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="str">
+        <f>VLOOKUP(A13,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>paymentPersonal</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="str">
+        <f>VLOOKUP(A14,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>taxPersonal</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="str">
+        <f>VLOOKUP(A15,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>taxProduction</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="str">
+        <f>VLOOKUP(A16,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>taxCorporate</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="str">
+        <f>VLOOKUP(A17,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>consumptionInvestment</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="str">
+        <f>VLOOKUP(A18,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>paymentSocialInsurance</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="str">
+        <f>VLOOKUP(A19,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>consumptionInvestmentFederal</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="str">
+        <f>VLOOKUP(A20,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>consumptionInvestmentState</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="str">
+        <f>VLOOKUP(A21,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>consumptionInvestmentRealState</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="str">
+        <f>VLOOKUP(A22,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>taxPersonalFederal</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="str">
+        <f>VLOOKUP(A23,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>taxProductionFederal</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="str">
+        <f>VLOOKUP(A24,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>taxCorporateFederal</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="str">
+        <f>VLOOKUP(A25,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>paymentSocialInsuranceFederal</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="str">
+        <f>VLOOKUP(A26,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>socialBenefitsFederal</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="str">
+        <f>VLOOKUP(A27,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>grantsFederal</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" t="str">
+        <f>VLOOKUP(A28,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>taxPersonalState</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" t="str">
+        <f>VLOOKUP(A29,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>taxProductionState</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="str">
+        <f>VLOOKUP(A30,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>taxCorporateState</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="str">
+        <f>VLOOKUP(A31,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>paymentSocialInsuranceState</v>
+      </c>
+      <c r="D31" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="str">
+        <f>VLOOKUP(A32,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>socialBenefitsState</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" t="str">
+        <f>VLOOKUP(A33,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>expendituresState</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="str">
+        <f>VLOOKUP(A34,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>subsidiesFederal</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" t="str">
+        <f>VLOOKUP(A35,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>consumptionInvestmentRealFederal</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" t="str">
+        <f>VLOOKUP(A36,'National Accounts Quarterly'!A:B,2,FALSE)</f>
+        <v>subsidiesState</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>234</v>
+      </c>
+      <c r="B37" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D0CC2C-8708-4348-BA01-659FDA1C3FDD}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB40C71-149D-46CE-B3DA-7A90274D8819}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC9F4DF-10CC-42D8-AE5E-BD4EE334E4EA}">
+  <dimension ref="A1:B110"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Gross Domestic Product (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="str">
+        <f>VLOOKUP(A3,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Personal Consumption Expenditures (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="str">
+        <f>VLOOKUP(A4,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Real Personal Consumption Expenditures (SAAR, Bil.Chn.2012.$) </v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="str">
+        <f>VLOOKUP(A5,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Real Gross Domestic Product (SAAR, Bil.Chn.2012$) </v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="str">
+        <f>VLOOKUP(A6,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Personal Consumption Expenditures: Chain Price Index (SA, 2012=100) </v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="str">
+        <f>VLOOKUP(A7,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Gross Domestic Product: Chain Price Index (SA, 2012=100) </v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" t="str">
+        <f>VLOOKUP(A8,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Govt Consumption &amp; Gross Investment: Chn Price Index(SA, 2012=100) </v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" t="str">
+        <f>VLOOKUP(A9,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Govt Consumption/Gross Investment: Chn Price Index(SA, 2012=100) </v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" t="str">
+        <f>VLOOKUP(A12,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Consumption &amp; Investment: Contrib to Real GDP % Change (SAAR, %Pt) </v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="str">
+        <f>VLOOKUP(A13,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Govt Consumption/Investment: Contrib to Real GDP % Chg (SAAR, %Pt) </v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" t="str">
+        <f>VLOOKUP(A14,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Govt Consumption &amp; Investment: Contrib to Real GDP % Change (SAAR, %Pt) </v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" t="str">
+        <f>VLOOKUP(A15,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Social Benefit Payments to Persons: Medicare (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" t="str">
+        <f>VLOOKUP(A16,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Social Benefit Payments to Persons: Medicaid (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" t="str">
+        <f>VLOOKUP(A17,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Govt Transf to Persons: Unemployment Insurance Benefits (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" t="str">
+        <f>VLOOKUP(A18,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Social Benefit Payments to Persons (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" t="str">
+        <f>VLOOKUP(A19,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Personal Current Transfer Payments to Government (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" t="str">
+        <f>VLOOKUP(A20,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Personal Current Taxes (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="str">
+        <f>VLOOKUP(A21,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" t="str">
+        <f>VLOOKUP(A22,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Tax Receipts on Corporate Income (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" t="str">
+        <f>VLOOKUP(A23,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Consumption Expenditures &amp; Gross Investment (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" t="str">
+        <f>VLOOKUP(A24,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Contributions for Government Social Insurance (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" t="str">
+        <f>VLOOKUP(A25,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Real Gross Domestic Product (SAAR, Bil.Chn.2012$) </v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" t="str">
+        <f>VLOOKUP(A26,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Personal Consumption Expenditures: Implicit Price Deflator (SA, 2012=100) </v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" t="str">
+        <f>VLOOKUP(A27,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Govt Consumption &amp; Investment: Contrib to Real GDP % Change (SAAR, %Pt) </v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" t="str">
+        <f>VLOOKUP(A28,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Govt Consumption/Investment: Contrib to Real GDP % Chg (SAAR, %Pt) </v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" t="str">
+        <f>VLOOKUP(A29,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Consumption &amp; Gross Investment (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" t="str">
+        <f>VLOOKUP(A30,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Government Consumption &amp; Gross Investment (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" t="str">
+        <f>VLOOKUP(A31,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Real Federal Government Consumption &amp; Gross Investment (SAAR, Bil.Chn.2012$) </v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" t="str">
+        <f>VLOOKUP(A32,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Real State &amp; Local Govt Consumption &amp; Gross Investment (SAAR, Bil.Chn.2012$) </v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" t="str">
+        <f>VLOOKUP(A33,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Personal Current Tax Receipts (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" t="str">
+        <f>VLOOKUP(A34,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" t="str">
+        <f>VLOOKUP(A35,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Tax Receipts on Corporate Income (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" t="str">
+        <f>VLOOKUP(A36,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Contributions for Federal Government Social Insurance (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" t="str">
+        <f>VLOOKUP(A37,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Personal Current Tax Receipts (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" t="str">
+        <f>VLOOKUP(A38,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" t="str">
+        <f>VLOOKUP(A39,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Tax Receipts on Corporate Income (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" t="str">
+        <f>VLOOKUP(A40,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Contributions for Federal Government Social Insurance (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" t="str">
+        <f>VLOOKUP(A41,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Social Benefit Payments to Persons (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" t="str">
+        <f>VLOOKUP(A42,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Grants-in-Aid to State &amp; Local Governments (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" t="str">
+        <f>VLOOKUP(A43,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Government Personal Current Tax Receipts (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" t="str">
+        <f>VLOOKUP(A44,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" t="str">
+        <f>VLOOKUP(A45,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Government Tax Receipts on Corporate Income (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>136</v>
+      </c>
+      <c r="B46" t="str">
+        <f>VLOOKUP(A46,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Contributions for State &amp; Local Government Social Insurance (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>137</v>
+      </c>
+      <c r="B47" t="str">
+        <f>VLOOKUP(A47,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Government Social Benefit Payments to Persons (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" t="str">
+        <f>VLOOKUP(A49,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v>Federal grants-in-aid to state and local governments: Health and Hospitals (SAAR, Mil.$)</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" t="str">
+        <f>VLOOKUP(A50,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v>Federal grants-in-aid to state and local governments: Medicaid (SAAR, Mil.$)</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>142</v>
+      </c>
+      <c r="B51" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>144</v>
+      </c>
+      <c r="B52" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>148</v>
+      </c>
+      <c r="B54" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>150</v>
+      </c>
+      <c r="B55" t="str">
+        <f>VLOOKUP(A55,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">CPI-W: All Items (SA, 1982-84=100) </v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" t="str">
+        <f>VLOOKUP(A56,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Real Potential Gross Domestic Product [CBO] (SAAR, Bil.Chn.2012$) </v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>152</v>
+      </c>
+      <c r="B57" t="str">
+        <f>VLOOKUP(A57,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Potential Gross Domestic Product [CBO] (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>153</v>
+      </c>
+      <c r="B58" t="str">
+        <f>VLOOKUP(A58,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v>Quarterly NBER Recession/Expansion: Recession Shading </v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" t="str">
+        <f>VLOOKUP(A60,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Gross Domestic Product (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" t="str">
+        <f>VLOOKUP(A61,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Personal Consumption Expenditures (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>99</v>
+      </c>
+      <c r="B62" t="str">
+        <f>VLOOKUP(A62,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Real Personal Consumption Expenditures (SAAR, Bil.Chn.2012.$) </v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>100</v>
+      </c>
+      <c r="B63" t="str">
+        <f>VLOOKUP(A63,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Real Gross Domestic Product (SAAR, Bil.Chn.2012$) </v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>101</v>
+      </c>
+      <c r="B64" t="str">
+        <f>VLOOKUP(A64,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Personal Consumption Expenditures: Chain Price Index (SA, 2012=100) </v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" t="str">
+        <f>VLOOKUP(A65,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Gross Domestic Product: Chain Price Index (SA, 2012=100) </v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" t="str">
+        <f>VLOOKUP(A66,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Govt Consumption &amp; Gross Investment: Chn Price Index(SA, 2012=100) </v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>104</v>
+      </c>
+      <c r="B67" t="str">
+        <f>VLOOKUP(A67,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Govt Consumption/Gross Investment: Chn Price Index(SA, 2012=100) </v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" t="str">
+        <f>VLOOKUP(A68,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Consumption &amp; Investment: Contrib to Real GDP % Change (SAAR, %Pt) </v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>110</v>
+      </c>
+      <c r="B69" t="str">
+        <f>VLOOKUP(A69,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Govt Consumption/Investment: Contrib to Real GDP % Chg (SAAR, %Pt) </v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70" t="str">
+        <f>VLOOKUP(A70,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Govt Consumption &amp; Investment: Contrib to Real GDP % Change (SAAR, %Pt) </v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>112</v>
+      </c>
+      <c r="B71" t="str">
+        <f>VLOOKUP(A71,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Social Benefit Payments to Persons: Medicare (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>113</v>
+      </c>
+      <c r="B72" t="str">
+        <f>VLOOKUP(A72,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Social Benefit Payments to Persons: Medicaid (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>115</v>
+      </c>
+      <c r="B73" t="str">
+        <f>VLOOKUP(A73,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Social Benefit Payments to Persons (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>116</v>
+      </c>
+      <c r="B74" t="str">
+        <f>VLOOKUP(A74,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Personal Current Transfer Payments to Government (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>117</v>
+      </c>
+      <c r="B75" t="str">
+        <f>VLOOKUP(A75,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Personal Current Taxes (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>118</v>
+      </c>
+      <c r="B76" t="str">
+        <f>VLOOKUP(A76,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>119</v>
+      </c>
+      <c r="B77" t="str">
+        <f>VLOOKUP(A77,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Tax Receipts on Corporate Income (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B78" t="str">
+        <f>VLOOKUP(A78,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Government Consumption Expenditures &amp; Gross Investment (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>121</v>
+      </c>
+      <c r="B79" t="str">
+        <f>VLOOKUP(A79,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Contributions for Government Social Insurance (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>100</v>
+      </c>
+      <c r="B80" t="str">
+        <f>VLOOKUP(A80,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Real Gross Domestic Product (SAAR, Bil.Chn.2012$) </v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>122</v>
+      </c>
+      <c r="B81" t="str">
+        <f>VLOOKUP(A81,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Personal Consumption Expenditures: Implicit Price Deflator (SA, 2012=100) </v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>111</v>
+      </c>
+      <c r="B82" t="str">
+        <f>VLOOKUP(A82,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Govt Consumption &amp; Investment: Contrib to Real GDP % Change (SAAR, %Pt) </v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>110</v>
+      </c>
+      <c r="B83" t="str">
+        <f>VLOOKUP(A83,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Govt Consumption/Investment: Contrib to Real GDP % Chg (SAAR, %Pt) </v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>123</v>
+      </c>
+      <c r="B84" t="str">
+        <f>VLOOKUP(A84,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Consumption &amp; Gross Investment (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>124</v>
+      </c>
+      <c r="B85" t="str">
+        <f>VLOOKUP(A85,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Government Consumption &amp; Gross Investment (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>125</v>
+      </c>
+      <c r="B86" t="str">
+        <f>VLOOKUP(A86,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Real Federal Government Consumption &amp; Gross Investment (SAAR, Bil.Chn.2012$) </v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>126</v>
+      </c>
+      <c r="B87" t="str">
+        <f>VLOOKUP(A87,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Real State &amp; Local Govt Consumption &amp; Gross Investment (SAAR, Bil.Chn.2012$) </v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>127</v>
+      </c>
+      <c r="B88" t="str">
+        <f>VLOOKUP(A88,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Personal Current Tax Receipts (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>128</v>
+      </c>
+      <c r="B89" t="str">
+        <f>VLOOKUP(A89,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>129</v>
+      </c>
+      <c r="B90" t="str">
+        <f>VLOOKUP(A90,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Tax Receipts on Corporate Income (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>130</v>
+      </c>
+      <c r="B91" t="str">
+        <f>VLOOKUP(A91,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Contributions for Federal Government Social Insurance (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>127</v>
+      </c>
+      <c r="B92" t="str">
+        <f>VLOOKUP(A92,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Personal Current Tax Receipts (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>128</v>
+      </c>
+      <c r="B93" t="str">
+        <f>VLOOKUP(A93,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>129</v>
+      </c>
+      <c r="B94" t="str">
+        <f>VLOOKUP(A94,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Tax Receipts on Corporate Income (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>130</v>
+      </c>
+      <c r="B95" t="str">
+        <f>VLOOKUP(A95,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Contributions for Federal Government Social Insurance (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>131</v>
+      </c>
+      <c r="B96" t="str">
+        <f>VLOOKUP(A96,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Government Social Benefit Payments to Persons (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>132</v>
+      </c>
+      <c r="B97" t="str">
+        <f>VLOOKUP(A97,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Federal Grants-in-Aid to State &amp; Local Governments (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>133</v>
+      </c>
+      <c r="B98" t="str">
+        <f>VLOOKUP(A98,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Government Personal Current Tax Receipts (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>134</v>
+      </c>
+      <c r="B99" t="str">
+        <f>VLOOKUP(A99,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Government Tax Receipts on Production &amp; Imports (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>135</v>
+      </c>
+      <c r="B100" t="str">
+        <f>VLOOKUP(A100,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Government Tax Receipts on Corporate Income (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>136</v>
+      </c>
+      <c r="B101" t="str">
+        <f>VLOOKUP(A101,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">Contributions for State &amp; Local Government Social Insurance (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>137</v>
+      </c>
+      <c r="B102" t="str">
+        <f>VLOOKUP(A102,[1]VLOOKUP!$A$1:$D$46,2,0)</f>
+        <v xml:space="preserve">State &amp; Local Government Social Benefit Payments to Persons (SAAR, Bil.$) </v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>138</v>
+      </c>
+      <c r="B103" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>155</v>
+      </c>
+      <c r="B104" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>144</v>
+      </c>
+      <c r="B105" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>146</v>
+      </c>
+      <c r="B106" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>157</v>
+      </c>
+      <c r="B107" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>159</v>
+      </c>
+      <c r="B108" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>161</v>
+      </c>
+      <c r="B109" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>163</v>
+      </c>
+      <c r="B110" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A59:B59"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941CCEA7-9E93-42C5-811A-D79E399AA88B}">
+  <dimension ref="A1:D46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10">
+        <v>2.1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11">
+        <v>2.1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C12">
+        <v>2.1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13">
+        <v>3.1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14">
+        <v>2.1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15">
+        <v>3.1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16">
+        <v>3.1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17">
+        <v>3.1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>189</v>
+      </c>
+      <c r="C18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" t="s">
+        <v>191</v>
+      </c>
+      <c r="D19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>192</v>
+      </c>
+      <c r="D20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21">
+        <v>3.1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>195</v>
+      </c>
+      <c r="C23" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C24" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>198</v>
+      </c>
+      <c r="C26">
+        <v>3.2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27">
+        <v>3.2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28">
+        <v>3.2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>201</v>
+      </c>
+      <c r="C29">
+        <v>3.2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
+        <v>202</v>
+      </c>
+      <c r="C30">
+        <v>3.2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" t="s">
+        <v>203</v>
+      </c>
+      <c r="C31">
+        <v>3.2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" t="s">
+        <v>204</v>
+      </c>
+      <c r="C32" t="s">
+        <v>205</v>
+      </c>
+      <c r="D32" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
+        <v>207</v>
+      </c>
+      <c r="C33" t="s">
+        <v>205</v>
+      </c>
+      <c r="D33" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>208</v>
+      </c>
+      <c r="B34" t="s">
+        <v>209</v>
+      </c>
+      <c r="C34" t="s">
+        <v>210</v>
+      </c>
+      <c r="D34" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>211</v>
+      </c>
+      <c r="C35">
+        <v>3.3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
+        <v>212</v>
+      </c>
+      <c r="C36">
+        <v>3.3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>213</v>
+      </c>
+      <c r="C37">
+        <v>3.3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>214</v>
+      </c>
+      <c r="C38">
+        <v>3.3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
+        <v>215</v>
+      </c>
+      <c r="C39">
+        <v>3.3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" t="s">
+        <v>216</v>
+      </c>
+      <c r="D40" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" t="s">
+        <v>217</v>
+      </c>
+      <c r="D41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" t="s">
+        <v>218</v>
+      </c>
+      <c r="D42" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>219</v>
+      </c>
+      <c r="B43" t="s">
+        <v>220</v>
+      </c>
+      <c r="D43" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>222</v>
+      </c>
+      <c r="B44" t="s">
+        <v>223</v>
+      </c>
+      <c r="D44" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>225</v>
+      </c>
+      <c r="B45" t="s">
+        <v>226</v>
+      </c>
+      <c r="D45" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>227</v>
+      </c>
+      <c r="B46" t="s">
+        <v>228</v>
+      </c>
+      <c r="D46" t="s">
+        <v>229</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D46" xr:uid="{1FE08E8B-D241-4522-9EF6-79D1FE87C0C9}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA9F3DB0CD4D844B918872BCED9B9CF9" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61f75d9b13a46a58fd2456a565edcb9c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cac5d118-ba7b-4807-b700-df6f95cfff50" xmlns:ns3="66951ee6-cd93-49c7-9437-e871b2a117d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d86870d415110e2c98f3a885b29630d1" ns2:_="" ns3:_="">
     <xsd:import namespace="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
@@ -1338,24 +4427,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C7CC3BF-DF9F-4E15-B3E2-3F2BE52E9D01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11C50A7A-072C-42B0-A807-112C623C860C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6FBE834-A7AF-4CA7-B4B3-E5BBA0B171E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1372,4 +4459,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11C50A7A-072C-42B0-A807-112C623C860C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C7CC3BF-DF9F-4E15-B3E2-3F2BE52E9D01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>